<commit_message>
Fixes inlezen parameterwaarden uit excels
-Aandelen heatingsystems worden nu goed uitgelezen uit de excelsheet wijkconfig. Verwees eerst naar sliders op de interface.
-Aandelen woningtypen en average label worden goed uitgelezen uit de excelsheet wijkconfig
-Buurtnamen toegevoegd zodat KPI-database goed ingevuld wordt.
</commit_message>
<xml_diff>
--- a/models/db_wijkconfig.xlsx
+++ b/models/db_wijkconfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\HOLON\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A943670F-615B-4B80-9F38-92B7C91F641E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A698DD60-23F3-450F-88E7-DE0AC7A25DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{98BF5335-066F-44F4-8DD0-240A4D27BDAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98BF5335-066F-44F4-8DD0-240A4D27BDAA}"/>
   </bookViews>
   <sheets>
     <sheet name="db_wijkconfig" sheetId="1" r:id="rId1"/>
@@ -463,15 +463,15 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -583,7 +583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -650,7 +650,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -664,9 +664,9 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -722,7 +722,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -778,7 +778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Cloud upload final version
- betrouwbaarheid staat op unknown
</commit_message>
<xml_diff>
--- a/models/db_wijkconfig.xlsx
+++ b/models/db_wijkconfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\HOLON\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A698DD60-23F3-450F-88E7-DE0AC7A25DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177E47FA-B8F7-4057-872B-C24C3D84D549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98BF5335-066F-44F4-8DD0-240A4D27BDAA}"/>
+    <workbookView xWindow="28680" yWindow="-945" windowWidth="29040" windowHeight="17640" xr2:uid="{98BF5335-066F-44F4-8DD0-240A4D27BDAA}"/>
   </bookViews>
   <sheets>
     <sheet name="db_wijkconfig" sheetId="1" r:id="rId1"/>
@@ -92,12 +92,6 @@
     <t>avg_motivation_sustainability</t>
   </si>
   <si>
-    <t>Buurt A: reguliere buurt</t>
-  </si>
-  <si>
-    <t>Buurt B: warmtenet</t>
-  </si>
-  <si>
     <t>B. Rijtjeswoningen</t>
   </si>
   <si>
@@ -108,6 +102,12 @@
   </si>
   <si>
     <t>A. Villawijk</t>
+  </si>
+  <si>
+    <t>Buurt A reguliere buurt</t>
+  </si>
+  <si>
+    <t>Buurt B warmtenet</t>
   </si>
 </sst>
 </file>
@@ -463,15 +463,15 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,12 +527,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1">
         <v>100</v>
@@ -583,12 +583,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1">
         <v>100</v>
@@ -650,7 +650,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -664,9 +664,9 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -722,12 +722,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1">
         <v>30</v>
@@ -778,12 +778,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1">
         <v>30</v>
@@ -834,12 +834,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1">
         <v>30</v>
@@ -890,12 +890,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1">
         <v>30</v>

</xml_diff>